<commit_message>
about to leave abu dhabi
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanfeng.Qin\Desktop\stellaris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96BCF55-FFF3-4FF8-A120-D202262A1273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CDF4EA-8F46-4CC4-A8A1-1EC8C3F91703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>output/job</t>
   </si>
   <si>
-    <t>trading benefits</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>Torpedo</t>
+  </si>
+  <si>
+    <t>trading benefits, exluding pop-number trade</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,7 +1041,7 @@
         <v>1.3359375</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1074,41 +1074,41 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5">
         <v>300</v>
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5">
         <f>IF(D4="S", 85, IF(D4="M", 215/2, 510/4))</f>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5">
         <v>800</v>
@@ -1157,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5">
         <f>IF(D5="S", 85, IF(D5="M", 215/2, 510/4))</f>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5">
         <v>1800</v>
@@ -1197,7 +1197,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5">
         <f>IF(D6="S", 85, IF(D6="M", 215/2, 510/4))</f>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5">
         <v>3000</v>
@@ -1237,7 +1237,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5">
         <f>IF(D7="S", 85, IF(D7="M", 215/2, 510/4))</f>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="5">
         <v>2000</v>
@@ -1277,7 +1277,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5">
         <f>IF(D8="S", 85, IF(D8="M", 215/2, 510/4))</f>
@@ -1332,13 +1332,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="7">
         <v>0.6</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1346,38 +1346,38 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5">
         <v>6.52</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5">
         <v>16.3</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
         <v>39.130000000000003</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="5">
         <v>45.7</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5">
         <v>145.83000000000001</v>
@@ -1528,36 +1528,36 @@
     <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -1701,17 +1701,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1756,60 +1756,60 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="O2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="Q2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="R2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="11">
         <v>15.45</v>
@@ -1860,10 +1860,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="11">
         <v>12.15</v>
@@ -1914,10 +1914,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="11">
         <v>6.22</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="11">
         <v>16.3</v>
@@ -2008,10 +2008,10 @@
     </row>
     <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="11">
         <v>6.82</v>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="11">
         <v>148.75</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="11">
         <v>105</v>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="11">
         <v>145.83000000000001</v>
@@ -2210,10 +2210,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="11">
         <v>42.41</v>
@@ -2264,10 +2264,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="11">
         <v>45.7</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="11">
         <v>11.41</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="11">
         <v>7.57</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="11">
         <v>3.46</v>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="11">
         <v>40</v>
@@ -2506,10 +2506,10 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="D17" s="11">
         <v>14.7</v>
@@ -2553,10 +2553,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="11">
         <v>17.059999999999999</v>
@@ -2600,12 +2600,12 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>